<commit_message>
Made changes in the data file
</commit_message>
<xml_diff>
--- a/src/test/java/com/Framework_with_cicd/TestData/Credentials.xlsx
+++ b/src/test/java/com/Framework_with_cicd/TestData/Credentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\eclipse-workspace\Framework_with_cicd\src\test\java\com\Framework_with_cicd\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D0367-F3C9-4FF8-AD67-0A872F43E057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1546D4AB-A3D3-40EB-A283-E1263B0A610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{21F86875-A413-4846-9BC3-3BF6FFBD54DC}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>asdf</t>
   </si>
@@ -55,13 +55,19 @@
     <t>Dokuparthi</t>
   </si>
   <si>
-    <t>Dokuparthi@gmail.com</t>
-  </si>
-  <si>
     <t>gkjgfkj123</t>
   </si>
   <si>
     <t>kjdfkjdf123</t>
+  </si>
+  <si>
+    <t>dokuparthi@gmail.com</t>
+  </si>
+  <si>
+    <t>123Dokuparthi</t>
+  </si>
+  <si>
+    <t>123fdsdfdf</t>
   </si>
 </sst>
 </file>
@@ -936,7 +942,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,10 +987,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -992,20 +998,20 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>12345</v>
-      </c>
-      <c r="D4">
-        <v>12345</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C43D2295-CE12-4A69-A627-821DD24DF698}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{ED5E2AA9-0C21-4290-BB59-6876D6D15083}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{A174F2E4-4E24-4616-807B-00AC73AA735B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{FCF6DCC7-CEA3-45F0-BE13-FE2F54AA6CFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>